<commit_message>
Add result.txt Signed-off-by: wuwenjun <591143357@qq.com>
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="38">
   <si>
     <t>randread:</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -101,39 +101,68 @@
     <t>Perf:</t>
   </si>
   <si>
+    <t>randread</t>
+  </si>
+  <si>
+    <t>runtime=300s</t>
+  </si>
+  <si>
+    <t>randwrite</t>
+  </si>
+  <si>
+    <t>runtime=600s</t>
+  </si>
+  <si>
+    <t>randrw</t>
+  </si>
+  <si>
     <t>randread:</t>
-  </si>
-  <si>
-    <t>randread</t>
-  </si>
-  <si>
-    <t>runtime=300s</t>
-  </si>
-  <si>
-    <t>randwrite</t>
-  </si>
-  <si>
-    <t>runtime=600s</t>
-  </si>
-  <si>
-    <t>randrw</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>K IOPS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1qd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4qd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>16qd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>K IOPS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Perf-AIO:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>128qd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -184,7 +213,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -200,7 +229,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -242,7 +271,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -277,7 +306,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -486,26 +515,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:L59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="2" width="11.375" customWidth="1"/>
+    <col min="3" max="3" width="9.875" customWidth="1"/>
+    <col min="6" max="6" width="9.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.15">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -518,7 +548,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -547,7 +577,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="13.5" customHeight="1">
+    <row r="4" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
@@ -576,12 +606,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.15">
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C5">
-        <v>1512</v>
+        <v>1425</v>
       </c>
       <c r="D5" t="s">
         <v>6</v>
@@ -605,7 +635,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="16.5" customHeight="1">
+    <row r="6" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
@@ -613,10 +643,10 @@
         <v>1670</v>
       </c>
       <c r="D6" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="G6" s="1">
         <v>1561</v>
@@ -634,16 +664,16 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15" customHeight="1"/>
-    <row r="8" spans="1:12">
+    <row r="7" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B8" s="1"/>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.15">
       <c r="B9" s="2" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>8</v>
@@ -652,7 +682,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.15">
       <c r="B10" t="s">
         <v>1</v>
       </c>
@@ -681,7 +711,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="14.25" customHeight="1">
+    <row r="11" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" t="s">
         <v>2</v>
       </c>
@@ -710,12 +740,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.15">
       <c r="B12" t="s">
         <v>4</v>
       </c>
       <c r="C12">
-        <v>102</v>
+        <v>179</v>
       </c>
       <c r="D12" t="s">
         <v>6</v>
@@ -739,7 +769,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.15">
       <c r="B13" t="s">
         <v>3</v>
       </c>
@@ -768,13 +798,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A15" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B15" s="1"/>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.15">
       <c r="B16" t="s">
         <v>0</v>
       </c>
@@ -785,7 +815,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.15">
       <c r="B17" t="s">
         <v>1</v>
       </c>
@@ -814,7 +844,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.15">
       <c r="B18" t="s">
         <v>2</v>
       </c>
@@ -843,7 +873,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.15">
       <c r="B19" t="s">
         <v>4</v>
       </c>
@@ -872,7 +902,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.15">
       <c r="B20" t="s">
         <v>3</v>
       </c>
@@ -901,78 +931,205 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
-      <c r="A22" t="s">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A23" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="1"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B24" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="J24" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25">
+        <v>109.2</v>
+      </c>
+      <c r="D25" t="s">
+        <v>35</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G25" s="1">
+        <v>87.2</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J25" t="s">
+        <v>1</v>
+      </c>
+      <c r="K25">
+        <v>73.3</v>
+      </c>
+      <c r="L25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B26" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26">
+        <v>370.1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>5</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G26" s="1">
+        <v>321.7</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J26" t="s">
+        <v>2</v>
+      </c>
+      <c r="K26">
+        <v>285.8</v>
+      </c>
+      <c r="L26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27">
+        <v>977.3</v>
+      </c>
+      <c r="D27" t="s">
+        <v>6</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G27" s="1">
+        <v>821.7</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J27" t="s">
+        <v>4</v>
+      </c>
+      <c r="K27">
+        <v>703.5</v>
+      </c>
+      <c r="L27" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B28" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" t="s">
+        <v>31</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J28" t="s">
+        <v>3</v>
+      </c>
+      <c r="L28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A47" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
-      <c r="A23" t="s">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A48" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
-      <c r="A24" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A49" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
-      <c r="A25" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A50" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
-      <c r="A26" t="s">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A51" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
-      <c r="A27" t="s">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A52" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
-      <c r="A28" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A53" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
-      <c r="A29" t="s">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A54" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
-      <c r="A30" t="s">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A55" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
-      <c r="A31" t="s">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A56" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:12">
-      <c r="A32" t="s">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A57" t="s">
+        <v>25</v>
+      </c>
+      <c r="B57" t="s">
         <v>26</v>
       </c>
-      <c r="B32" t="s">
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A58" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" t="s">
+      <c r="B58" t="s">
         <v>28</v>
       </c>
-      <c r="B33" t="s">
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A59" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" t="s">
-        <v>30</v>
-      </c>
-      <c r="B34" t="s">
-        <v>29</v>
+      <c r="B59" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add excl Signed-off-by: wuwenjun <591143357@qq.com>
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="195" windowWidth="14805" windowHeight="7920"/>
   </bookViews>
   <sheets>
     <sheet name="IOPS " sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="48">
   <si>
     <t>randread:</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -145,6 +145,46 @@
   </si>
   <si>
     <t>128qd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>128qd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>randread:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1qd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>K IOPS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Clat:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4qd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>16qd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>randread_1qd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>randwrite_1qd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Clat/kernel:</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -168,7 +208,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -193,6 +233,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -206,11 +252,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -515,18 +564,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L59"/>
+  <dimension ref="A1:L83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="11.375" customWidth="1"/>
-    <col min="3" max="3" width="9.875" customWidth="1"/>
-    <col min="6" max="6" width="9.75" customWidth="1"/>
+    <col min="2" max="2" width="13.625" customWidth="1"/>
+    <col min="3" max="3" width="14.375" customWidth="1"/>
+    <col min="4" max="4" width="12.375" customWidth="1"/>
+    <col min="6" max="6" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.15">
@@ -637,7 +687,7 @@
     </row>
     <row r="6" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="1" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="C6">
         <v>1670</v>
@@ -655,7 +705,7 @@
         <v>5</v>
       </c>
       <c r="J6" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="K6">
         <v>891</v>
@@ -696,7 +746,7 @@
         <v>1</v>
       </c>
       <c r="G10">
-        <v>14.3</v>
+        <v>100.8</v>
       </c>
       <c r="H10" t="s">
         <v>5</v>
@@ -728,7 +778,7 @@
         <v>50.4</v>
       </c>
       <c r="H11" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="J11" t="s">
         <v>2</v>
@@ -771,16 +821,16 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.15">
       <c r="B13" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="C13">
         <v>1211</v>
       </c>
       <c r="D13" t="s">
-        <v>5</v>
+        <v>41</v>
       </c>
       <c r="F13" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="G13">
         <v>1109</v>
@@ -817,7 +867,7 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.15">
       <c r="B17" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="C17">
         <v>89.4</v>
@@ -904,7 +954,7 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.15">
       <c r="B20" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="C20">
         <v>2456.4</v>
@@ -939,7 +989,7 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.15">
       <c r="B24" s="2" t="s">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>8</v>
@@ -1039,7 +1089,10 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.15">
       <c r="B28" t="s">
-        <v>3</v>
+        <v>38</v>
+      </c>
+      <c r="C28">
+        <v>1421.6</v>
       </c>
       <c r="D28" t="s">
         <v>31</v>
@@ -1047,93 +1100,435 @@
       <c r="F28" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G28" s="1"/>
+      <c r="G28" s="1">
+        <v>1326.4</v>
+      </c>
       <c r="H28" s="1" t="s">
         <v>5</v>
       </c>
       <c r="J28" t="s">
         <v>3</v>
       </c>
+      <c r="K28">
+        <v>856.3</v>
+      </c>
       <c r="L28" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A47" t="s">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A31" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A32" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="C32">
+        <v>36</v>
+      </c>
+      <c r="D32">
+        <v>57</v>
+      </c>
+      <c r="F32" s="1"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A33" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="B33">
+        <v>109.2</v>
+      </c>
+      <c r="C33">
+        <v>83</v>
+      </c>
+      <c r="D33" s="1">
+        <v>89</v>
+      </c>
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A34" s="5">
+        <v>0.99</v>
+      </c>
+      <c r="B34">
+        <v>370.1</v>
+      </c>
+      <c r="C34">
+        <v>98</v>
+      </c>
+      <c r="D34" s="1">
+        <v>123</v>
+      </c>
+      <c r="E34" s="1"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A35" s="4">
+        <v>0.999</v>
+      </c>
+      <c r="B35">
+        <v>977.3</v>
+      </c>
+      <c r="C35">
+        <v>506</v>
+      </c>
+      <c r="D35" s="1">
+        <v>556</v>
+      </c>
+      <c r="E35" s="1"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A36" s="4">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="C36">
+        <v>2768</v>
+      </c>
+      <c r="D36" s="1">
+        <v>2768</v>
+      </c>
+      <c r="E36" s="1"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A38" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A39" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="B39" s="1">
+        <v>6</v>
+      </c>
+      <c r="C39">
+        <v>6</v>
+      </c>
+      <c r="D39" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A40" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="B40">
+        <v>7</v>
+      </c>
+      <c r="C40">
+        <v>7</v>
+      </c>
+      <c r="D40" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A41" s="5">
+        <v>0.99</v>
+      </c>
+      <c r="B41">
+        <v>9</v>
+      </c>
+      <c r="C41">
+        <v>9</v>
+      </c>
+      <c r="D41" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A42" s="4">
+        <v>0.999</v>
+      </c>
+      <c r="B42">
+        <v>22</v>
+      </c>
+      <c r="C42">
+        <v>23</v>
+      </c>
+      <c r="D42" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A43" s="4">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="B43">
+        <v>45</v>
+      </c>
+      <c r="C43">
+        <v>45</v>
+      </c>
+      <c r="D43" s="1">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A45" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A46" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="B46" s="1">
+        <v>50</v>
+      </c>
+      <c r="C46">
+        <v>57</v>
+      </c>
+      <c r="D46">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A47" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="B47">
+        <v>85</v>
+      </c>
+      <c r="C47">
+        <v>86</v>
+      </c>
+      <c r="D47" s="1">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A48" s="5">
+        <v>0.99</v>
+      </c>
+      <c r="B48">
+        <v>129</v>
+      </c>
+      <c r="C48">
+        <v>129</v>
+      </c>
+      <c r="D48" s="1">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A49" s="4">
+        <v>0.999</v>
+      </c>
+      <c r="B49">
+        <v>157</v>
+      </c>
+      <c r="C49">
+        <v>201</v>
+      </c>
+      <c r="D49" s="1">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A50" s="4">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="B50">
+        <v>330</v>
+      </c>
+      <c r="C50">
+        <v>780</v>
+      </c>
+      <c r="D50" s="1">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A52" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A53" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="B53" s="1">
+        <v>12</v>
+      </c>
+      <c r="C53">
+        <v>15</v>
+      </c>
+      <c r="D53">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A54" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="B54">
+        <v>13</v>
+      </c>
+      <c r="C54">
+        <v>20</v>
+      </c>
+      <c r="D54" s="1">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A55" s="5">
+        <v>0.99</v>
+      </c>
+      <c r="B55">
         <v>21</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A48" t="s">
+      <c r="C55">
+        <v>38</v>
+      </c>
+      <c r="D55" s="1">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A56" s="4">
+        <v>0.999</v>
+      </c>
+      <c r="B56">
+        <v>34</v>
+      </c>
+      <c r="C56">
+        <v>76</v>
+      </c>
+      <c r="D56" s="1">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A57" s="4">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="B57">
+        <v>53</v>
+      </c>
+      <c r="C57">
+        <v>135</v>
+      </c>
+      <c r="D57" s="1">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A71" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A72" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A49" t="s">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A73" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A50" t="s">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A74" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A51" t="s">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A75" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A52" t="s">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A76" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A53" t="s">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A77" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A54" t="s">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A78" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A55" t="s">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A79" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A56" t="s">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A80" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A57" t="s">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A81" t="s">
         <v>25</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B81" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A58" t="s">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A82" t="s">
         <v>27</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B82" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A59" t="s">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A83" t="s">
         <v>29</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B83" t="s">
         <v>28</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>